<commit_message>
late commit - updated tables and READme before submitted to JEB
</commit_message>
<xml_diff>
--- a/RAnalysis/Sample.Tracker/Sample.Tracker.FINAL.assay.checklist.xlsx
+++ b/RAnalysis/Sample.Tracker/Sample.Tracker.FINAL.assay.checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Inragenerational_thresholds_OA\RAnalysis\Sample.Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2ED382-82CB-434F-ABE0-C8EBAB9D6988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B051F5-E33A-4DA8-BCBC-A2DC56F0510E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="195" windowWidth="19755" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample.Tracker.FINAL" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10149" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10156" uniqueCount="199">
   <si>
     <t>Tube.ID</t>
   </si>
@@ -1519,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1645"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A377" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I390" sqref="I390"/>
+    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N382" sqref="A372:N382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14875,37 +14875,42 @@
       </c>
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A357" s="3">
+      <c r="A357" s="14">
         <v>296</v>
       </c>
-      <c r="B357" s="3">
+      <c r="B357" s="14">
         <v>20190728</v>
       </c>
-      <c r="C357" s="3">
+      <c r="C357" s="14">
         <v>30</v>
       </c>
-      <c r="D357" s="3" t="s">
+      <c r="D357" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E357" s="3">
+      <c r="E357" s="14">
         <v>3</v>
       </c>
-      <c r="F357" s="3" t="s">
+      <c r="F357" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G357" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H357" s="3" t="s">
+      <c r="G357" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H357" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J357" s="3" t="s">
+      <c r="I357" s="14"/>
+      <c r="J357" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K357" s="3" t="s">
+      <c r="K357" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="N357" s="3">
+      <c r="L357" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M357" s="14"/>
+      <c r="N357" s="14">
         <v>296</v>
       </c>
     </row>
@@ -14945,37 +14950,42 @@
       </c>
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A359" s="3">
+      <c r="A359" s="14">
         <v>308</v>
       </c>
-      <c r="B359" s="3">
+      <c r="B359" s="14">
         <v>20190728</v>
       </c>
-      <c r="C359" s="3">
+      <c r="C359" s="14">
         <v>33</v>
       </c>
-      <c r="D359" s="3" t="s">
+      <c r="D359" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E359" s="3">
+      <c r="E359" s="14">
         <v>3</v>
       </c>
-      <c r="F359" s="3" t="s">
+      <c r="F359" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G359" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H359" s="3" t="s">
+      <c r="G359" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H359" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J359" s="3" t="s">
+      <c r="I359" s="14"/>
+      <c r="J359" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K359" s="3" t="s">
+      <c r="K359" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="N359" s="3">
+      <c r="L359" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M359" s="14"/>
+      <c r="N359" s="14">
         <v>308</v>
       </c>
     </row>
@@ -15155,37 +15165,42 @@
       </c>
     </row>
     <row r="365" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A365" s="3">
+      <c r="A365" s="14">
         <v>312</v>
       </c>
-      <c r="B365" s="3">
+      <c r="B365" s="14">
         <v>20190728</v>
       </c>
-      <c r="C365" s="3">
+      <c r="C365" s="14">
         <v>34</v>
       </c>
-      <c r="D365" s="3" t="s">
+      <c r="D365" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E365" s="3">
+      <c r="E365" s="14">
         <v>3</v>
       </c>
-      <c r="F365" s="3" t="s">
+      <c r="F365" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G365" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H365" s="3" t="s">
+      <c r="G365" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H365" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J365" s="3" t="s">
+      <c r="I365" s="14"/>
+      <c r="J365" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="K365" s="3" t="s">
+      <c r="K365" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N365" s="3">
+      <c r="L365" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M365" s="14"/>
+      <c r="N365" s="14">
         <v>312</v>
       </c>
     </row>
@@ -15260,37 +15275,42 @@
       </c>
     </row>
     <row r="368" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A368" s="3">
+      <c r="A368" s="14">
         <v>318</v>
       </c>
-      <c r="B368" s="3">
+      <c r="B368" s="14">
         <v>20190728</v>
       </c>
-      <c r="C368" s="3">
+      <c r="C368" s="14">
         <v>36</v>
       </c>
-      <c r="D368" s="3" t="s">
+      <c r="D368" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E368" s="3">
-        <v>1</v>
-      </c>
-      <c r="F368" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G368" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H368" s="3" t="s">
+      <c r="E368" s="14">
+        <v>1</v>
+      </c>
+      <c r="F368" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G368" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H368" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J368" s="3" t="s">
+      <c r="I368" s="14"/>
+      <c r="J368" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="K368" s="3" t="s">
+      <c r="K368" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N368" s="3">
+      <c r="L368" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M368" s="14"/>
+      <c r="N368" s="14">
         <v>318</v>
       </c>
     </row>
@@ -15400,37 +15420,40 @@
       </c>
     </row>
     <row r="372" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A372" s="3">
+      <c r="A372" s="14">
         <v>190</v>
       </c>
-      <c r="B372" s="3">
+      <c r="B372" s="14">
         <v>20190728</v>
       </c>
-      <c r="C372" s="3">
+      <c r="C372" s="14">
         <v>4</v>
       </c>
-      <c r="D372" s="3" t="s">
+      <c r="D372" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E372" s="3">
-        <v>1</v>
-      </c>
-      <c r="F372" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G372" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H372" s="3" t="s">
+      <c r="E372" s="14">
+        <v>1</v>
+      </c>
+      <c r="F372" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G372" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H372" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J372" s="3" t="s">
+      <c r="I372" s="14"/>
+      <c r="J372" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="K372" s="3" t="s">
+      <c r="K372" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N372" s="3">
+      <c r="L372" s="14"/>
+      <c r="M372" s="14"/>
+      <c r="N372" s="14">
         <v>190</v>
       </c>
     </row>
@@ -15470,37 +15493,40 @@
       </c>
     </row>
     <row r="374" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A374" s="3">
+      <c r="A374" s="14">
         <v>196</v>
       </c>
-      <c r="B374" s="3">
+      <c r="B374" s="14">
         <v>20190728</v>
       </c>
-      <c r="C374" s="3">
+      <c r="C374" s="14">
         <v>5</v>
       </c>
-      <c r="D374" s="3" t="s">
+      <c r="D374" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E374" s="3">
+      <c r="E374" s="14">
         <v>3</v>
       </c>
-      <c r="F374" s="3" t="s">
+      <c r="F374" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G374" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H374" s="3" t="s">
+      <c r="G374" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H374" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J374" s="3" t="s">
+      <c r="I374" s="14"/>
+      <c r="J374" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K374" s="3" t="s">
+      <c r="K374" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N374" s="3">
+      <c r="L374" s="14"/>
+      <c r="M374" s="14"/>
+      <c r="N374" s="14">
         <v>196</v>
       </c>
     </row>
@@ -15610,37 +15636,40 @@
       </c>
     </row>
     <row r="378" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A378" s="3">
+      <c r="A378" s="14">
         <v>200</v>
       </c>
-      <c r="B378" s="3">
+      <c r="B378" s="14">
         <v>20190728</v>
       </c>
-      <c r="C378" s="3">
+      <c r="C378" s="14">
         <v>6</v>
       </c>
-      <c r="D378" s="3" t="s">
+      <c r="D378" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E378" s="3">
+      <c r="E378" s="14">
         <v>3</v>
       </c>
-      <c r="F378" s="3" t="s">
+      <c r="F378" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G378" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H378" s="3" t="s">
+      <c r="G378" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H378" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J378" s="3" t="s">
+      <c r="I378" s="14"/>
+      <c r="J378" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="K378" s="3" t="s">
+      <c r="K378" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N378" s="3">
+      <c r="L378" s="14"/>
+      <c r="M378" s="14"/>
+      <c r="N378" s="14">
         <v>200</v>
       </c>
     </row>
@@ -15750,40 +15779,40 @@
       </c>
     </row>
     <row r="382" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A382" s="3">
+      <c r="A382" s="14">
         <v>216</v>
       </c>
-      <c r="B382" s="3">
+      <c r="B382" s="14">
         <v>20190728</v>
       </c>
-      <c r="C382" s="3">
+      <c r="C382" s="14">
         <v>10</v>
       </c>
-      <c r="D382" s="3" t="s">
+      <c r="D382" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E382" s="3">
+      <c r="E382" s="14">
         <v>3</v>
       </c>
-      <c r="F382" s="3" t="s">
+      <c r="F382" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G382" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H382" s="3" t="s">
+      <c r="G382" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H382" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I382" s="3"/>
-      <c r="J382" s="3" t="s">
+      <c r="I382" s="14"/>
+      <c r="J382" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="K382" s="3" t="s">
+      <c r="K382" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="L382" s="3"/>
-      <c r="M382" s="3"/>
-      <c r="N382" s="3">
+      <c r="L382" s="14"/>
+      <c r="M382" s="14"/>
+      <c r="N382" s="14">
         <v>216</v>
       </c>
       <c r="O382" s="3"/>
@@ -17268,40 +17297,42 @@
       </c>
     </row>
     <row r="424" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A424" s="3">
+      <c r="A424" s="14">
         <v>291</v>
       </c>
-      <c r="B424" s="3">
+      <c r="B424" s="14">
         <v>20190728</v>
       </c>
-      <c r="C424" s="3">
+      <c r="C424" s="14">
         <v>29</v>
       </c>
-      <c r="D424" s="3" t="s">
+      <c r="D424" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E424" s="3">
-        <v>1</v>
-      </c>
-      <c r="F424" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G424" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H424" s="3" t="s">
+      <c r="E424" s="14">
+        <v>1</v>
+      </c>
+      <c r="F424" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G424" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H424" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I424" s="3"/>
-      <c r="J424" s="3" t="s">
+      <c r="I424" s="14"/>
+      <c r="J424" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K424" s="3" t="s">
+      <c r="K424" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L424" s="3"/>
-      <c r="M424" s="3"/>
-      <c r="N424" s="3">
+      <c r="L424" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M424" s="14"/>
+      <c r="N424" s="14">
         <v>291</v>
       </c>
       <c r="O424" s="3"/>
@@ -17420,76 +17451,83 @@
       </c>
     </row>
     <row r="428" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A428" s="3">
+      <c r="A428" s="14">
         <v>300</v>
       </c>
-      <c r="B428" s="3">
+      <c r="B428" s="14">
         <v>20190728</v>
       </c>
-      <c r="C428" s="3">
+      <c r="C428" s="14">
         <v>31</v>
       </c>
-      <c r="D428" s="3" t="s">
+      <c r="D428" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E428" s="3">
+      <c r="E428" s="14">
         <v>3</v>
       </c>
-      <c r="F428" s="3" t="s">
+      <c r="F428" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G428" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H428" s="3" t="s">
+      <c r="G428" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H428" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="I428" s="3"/>
-      <c r="J428" s="3" t="s">
+      <c r="I428" s="14"/>
+      <c r="J428" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="K428" s="3" t="s">
+      <c r="K428" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L428" s="3"/>
-      <c r="M428" s="3"/>
-      <c r="N428" s="3">
+      <c r="L428" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M428" s="14"/>
+      <c r="N428" s="14">
         <v>300</v>
       </c>
       <c r="O428" s="3"/>
     </row>
     <row r="429" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A429" s="3">
+      <c r="A429" s="14">
         <v>304</v>
       </c>
-      <c r="B429" s="3">
+      <c r="B429" s="14">
         <v>20190728</v>
       </c>
-      <c r="C429" s="3">
+      <c r="C429" s="14">
         <v>32</v>
       </c>
-      <c r="D429" s="3" t="s">
+      <c r="D429" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E429" s="3">
+      <c r="E429" s="14">
         <v>3</v>
       </c>
-      <c r="F429" s="3" t="s">
+      <c r="F429" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G429" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H429" s="3" t="s">
+      <c r="G429" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H429" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J429" s="3" t="s">
+      <c r="I429" s="14"/>
+      <c r="J429" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K429" s="3" t="s">
+      <c r="K429" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N429" s="3">
+      <c r="L429" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M429" s="14"/>
+      <c r="N429" s="14">
         <v>304</v>
       </c>
     </row>
@@ -17673,37 +17711,42 @@
       </c>
     </row>
     <row r="435" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A435" s="3">
+      <c r="A435" s="14">
         <v>316</v>
       </c>
-      <c r="B435" s="3">
+      <c r="B435" s="14">
         <v>20190728</v>
       </c>
-      <c r="C435" s="3">
+      <c r="C435" s="14">
         <v>35</v>
       </c>
-      <c r="D435" s="3" t="s">
+      <c r="D435" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E435" s="3">
+      <c r="E435" s="14">
         <v>3</v>
       </c>
-      <c r="F435" s="3" t="s">
+      <c r="F435" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G435" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H435" s="3" t="s">
+      <c r="G435" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H435" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="J435" s="3" t="s">
+      <c r="I435" s="14"/>
+      <c r="J435" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="K435" s="3" t="s">
+      <c r="K435" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="N435" s="3">
+      <c r="L435" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="M435" s="14"/>
+      <c r="N435" s="14">
         <v>316</v>
       </c>
     </row>
@@ -31650,42 +31693,37 @@
       </c>
     </row>
     <row r="830" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A830" s="14">
+      <c r="A830" s="3">
         <v>675</v>
       </c>
-      <c r="B830" s="14">
+      <c r="B830" s="3">
         <v>20190804</v>
       </c>
-      <c r="C830" s="14">
+      <c r="C830" s="3">
         <v>23</v>
       </c>
-      <c r="D830" s="14" t="s">
+      <c r="D830" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E830" s="14">
-        <v>1</v>
-      </c>
-      <c r="F830" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G830" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H830" s="14" t="s">
+      <c r="E830" s="3">
+        <v>1</v>
+      </c>
+      <c r="F830" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G830" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H830" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I830" s="14"/>
-      <c r="J830" s="14" t="s">
+      <c r="J830" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="K830" s="14" t="s">
+      <c r="K830" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L830" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="M830" s="14"/>
-      <c r="N830" s="14">
+      <c r="N830" s="3">
         <v>675</v>
       </c>
     </row>

</xml_diff>